<commit_message>
Fixed but in analysis.py for rotation detection.
</commit_message>
<xml_diff>
--- a/Notes.xlsx
+++ b/Notes.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28908"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="29005"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/akulesa/Desktop/kChip Code/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/akulesa/Desktop/20180310/kchip/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="4060" yWindow="460" windowWidth="28800" windowHeight="17460" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="7440" yWindow="920" windowWidth="28800" windowHeight="17460" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Barcodes" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="60">
   <si>
     <t>A</t>
   </si>
@@ -78,62 +78,143 @@
     <t>Col8</t>
   </si>
   <si>
-    <t>[3,0,0]</t>
-  </si>
-  <si>
-    <t>[0,3,0]</t>
-  </si>
-  <si>
-    <t>[0, 0, 3]</t>
-  </si>
-  <si>
-    <t>[2, 1, 0]</t>
-  </si>
-  <si>
-    <t>[2, 0.5, 0.5]</t>
-  </si>
-  <si>
-    <t>[2, 0, 1]</t>
-  </si>
-  <si>
-    <t>[0, 2, 1]</t>
-  </si>
-  <si>
-    <t>[0.5, 2, 0.5]</t>
-  </si>
-  <si>
-    <t>[1, 2, 0]</t>
-  </si>
-  <si>
-    <t>[1, 0, 2]</t>
-  </si>
-  <si>
-    <t>[0.5, 0.5, 2]</t>
-  </si>
-  <si>
-    <t>[0, 1, 2]</t>
-  </si>
-  <si>
-    <t>[1.5, 1, 0.5]</t>
-  </si>
-  <si>
-    <t>[0, 1.5, 1]</t>
-  </si>
-  <si>
-    <t>[1, 0, 1.5]</t>
-  </si>
-  <si>
-    <t>[1, 1, 1]</t>
-  </si>
-  <si>
-    <t>I</t>
+    <t>MF-H8</t>
+  </si>
+  <si>
+    <t>KC-A8</t>
+  </si>
+  <si>
+    <t>KC-H1</t>
+  </si>
+  <si>
+    <t>KC-C2</t>
+  </si>
+  <si>
+    <t>KC-H2</t>
+  </si>
+  <si>
+    <t>KC-C7</t>
+  </si>
+  <si>
+    <t>KC-H4</t>
+  </si>
+  <si>
+    <t>KC-D5</t>
+  </si>
+  <si>
+    <t>KC-H9</t>
+  </si>
+  <si>
+    <t>KC-E1</t>
+  </si>
+  <si>
+    <t>MF-A11</t>
+  </si>
+  <si>
+    <t>KC-E3</t>
+  </si>
+  <si>
+    <t>MF-B10</t>
+  </si>
+  <si>
+    <t>KC-F4</t>
+  </si>
+  <si>
+    <t>MF-F4</t>
+  </si>
+  <si>
+    <t>KC-F7</t>
+  </si>
+  <si>
+    <t>MF-G8</t>
+  </si>
+  <si>
+    <t>Pp-u</t>
+  </si>
+  <si>
+    <t>Nor</t>
+  </si>
+  <si>
+    <t>LB1</t>
+  </si>
+  <si>
+    <t>LB2</t>
+  </si>
+  <si>
+    <t>LB3</t>
+  </si>
+  <si>
+    <t>[0,50,0]</t>
+  </si>
+  <si>
+    <t>[1,0,49]</t>
+  </si>
+  <si>
+    <t>[1,4,45]</t>
+  </si>
+  <si>
+    <t>[3,29,18]</t>
+  </si>
+  <si>
+    <t>[3,33,13]</t>
+  </si>
+  <si>
+    <t>[4,38,9]</t>
+  </si>
+  <si>
+    <t>[7,17,27]</t>
+  </si>
+  <si>
+    <t>[7,21,22]</t>
+  </si>
+  <si>
+    <t>[7,25,18]</t>
+  </si>
+  <si>
+    <t>[10,8,31]</t>
+  </si>
+  <si>
+    <t>[11,13,27]</t>
+  </si>
+  <si>
+    <t>[11,17,22]</t>
+  </si>
+  <si>
+    <t>[15,4,31]</t>
+  </si>
+  <si>
+    <t>[15,8,27]</t>
+  </si>
+  <si>
+    <t>[15,13,22]</t>
+  </si>
+  <si>
+    <t>[19,4,27]</t>
+  </si>
+  <si>
+    <t>[20,8,22]</t>
+  </si>
+  <si>
+    <t>[20,13,18]</t>
+  </si>
+  <si>
+    <t>[24,8,17]</t>
+  </si>
+  <si>
+    <t>[25,13,13]</t>
+  </si>
+  <si>
+    <t>[29,17,4]</t>
+  </si>
+  <si>
+    <t>[33,0,17]</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -171,14 +252,10 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="12"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -211,13 +288,12 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="11">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -507,8 +583,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -543,67 +619,53 @@
       <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="I2" s="4" t="s">
-        <v>23</v>
-      </c>
+      <c r="B2" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="E3" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="F3" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="G3" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="H3" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="I3" s="5" t="s">
-        <v>31</v>
-      </c>
+      <c r="B3" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
+      <c r="B4" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>46</v>
+      </c>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
@@ -614,9 +676,15 @@
       <c r="A5" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
+      <c r="B5" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>49</v>
+      </c>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
@@ -627,9 +695,15 @@
       <c r="A6" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
+      <c r="B6" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>52</v>
+      </c>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
@@ -640,9 +714,15 @@
       <c r="A7" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
+      <c r="B7" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>55</v>
+      </c>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
@@ -653,8 +733,12 @@
       <c r="A8" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
+      <c r="B8" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>57</v>
+      </c>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
@@ -666,8 +750,12 @@
       <c r="A9" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
+      <c r="B9" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>59</v>
+      </c>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
@@ -683,10 +771,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I9"/>
+  <dimension ref="A1:I19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -722,46 +810,48 @@
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
+      <c r="B2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" t="s">
+        <v>18</v>
+      </c>
       <c r="D2" t="s">
-        <v>32</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>1</v>
+      <c r="B3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" t="s">
+        <v>20</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>7</v>
-      </c>
+        <v>33</v>
+      </c>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
+      <c r="B4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>34</v>
+      </c>
       <c r="E4" s="3"/>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
@@ -772,9 +862,15 @@
       <c r="A5" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
+      <c r="B5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>35</v>
+      </c>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
@@ -785,9 +881,15 @@
       <c r="A6" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
+      <c r="B6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>36</v>
+      </c>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
@@ -798,9 +900,15 @@
       <c r="A7" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
+      <c r="B7" t="s">
+        <v>27</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>37</v>
+      </c>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
@@ -811,8 +919,12 @@
       <c r="A8" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
+      <c r="B8" t="s">
+        <v>29</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>30</v>
+      </c>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
@@ -824,8 +936,12 @@
       <c r="A9" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
+      <c r="B9" t="s">
+        <v>31</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>32</v>
+      </c>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
@@ -833,6 +949,41 @@
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
     </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B11" s="4"/>
+      <c r="C11" s="4"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B12" s="4"/>
+      <c r="C12" s="4"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B13" s="4"/>
+      <c r="C13" s="4"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B14" s="4"/>
+      <c r="C14" s="4"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B15" s="4"/>
+      <c r="C15" s="4"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B16" s="4"/>
+      <c r="C16" s="4"/>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B17" s="4"/>
+      <c r="C17" s="4"/>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B18" s="4"/>
+      <c r="C18" s="4"/>
+    </row>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="C19" s="4"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>